<commit_message>
Updated Change History tracker
</commit_message>
<xml_diff>
--- a/LLM/EquityResearchReports/ER_Change_History.xlsx
+++ b/LLM/EquityResearchReports/ER_Change_History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shriniwasiyengar/git/python_ML/LLM/EquityResearchReports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BCA4FD-4756-CB43-94F8-A17F5A7B9A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7985EBF-CE7F-8647-A509-88D1B76620BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" xr2:uid="{F111C49C-E983-B94D-AD50-206753B053C1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="84">
   <si>
     <t>CR or Bug #</t>
   </si>
@@ -309,22 +309,21 @@
   <si>
     <t>CR0023</t>
   </si>
+  <si>
+    <t>Used sqlite embedded database as a lightweight solution to store source data info. Added corresponding source management components into frontend and backend. The frontend source management component interacts with the company dropdown via Angular events.Frontend users tabs to show sources etc.</t>
+  </si>
+  <si>
+    <t>Added IA reports service components in frontend and backend. Frontend uses tabs to show IA report, chat, sources etc. The backed IA service runs in the same docker container as the chat service but on a different port.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -384,7 +383,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -399,7 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -719,7 +718,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,7 +803,7 @@
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -825,7 +824,9 @@
       <c r="G4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="3"/>
+      <c r="H4" s="8" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
@@ -850,7 +851,7 @@
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -871,7 +872,9 @@
       <c r="G6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2">

</xml_diff>

<commit_message>
BUG0002:Sources were not being added / updated properly. Dropdown box was not showing active sources.
</commit_message>
<xml_diff>
--- a/LLM/EquityResearchReports/ER_Change_History.xlsx
+++ b/LLM/EquityResearchReports/ER_Change_History.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shriniwasiyengar/git/python_ML/LLM/EquityResearchReports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7985EBF-CE7F-8647-A509-88D1B76620BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C278662-771B-2E4A-BEC0-C66B62E6266D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" xr2:uid="{F111C49C-E983-B94D-AD50-206753B053C1}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{F111C49C-E983-B94D-AD50-206753B053C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="87">
   <si>
     <t>CR or Bug #</t>
   </si>
@@ -314,6 +314,15 @@
   </si>
   <si>
     <t>Added IA reports service components in frontend and backend. Frontend uses tabs to show IA report, chat, sources etc. The backed IA service runs in the same docker container as the chat service but on a different port.</t>
+  </si>
+  <si>
+    <t>BUG0002</t>
+  </si>
+  <si>
+    <t>Sources were not being added / updated properly. Dropdown box was not showing active sources.</t>
+  </si>
+  <si>
+    <t>Created additional endpoints in Sources Management Service. Added new event for getting companies list. Added separate Sources_URL environment variable.</t>
   </si>
 </sst>
 </file>
@@ -375,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -401,6 +410,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3DE150-7B8A-A542-8341-29F2F94982DD}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -757,76 +770,76 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <f t="shared" ref="A2:A8" si="0">ROW()-1</f>
+    <row r="2" spans="1:8" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <f t="shared" ref="A2:A9" si="0">ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>46</v>
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
+      <c r="B4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>82</v>
-      </c>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
@@ -834,80 +847,80 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>76</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="2" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="H5" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>8</v>
+      <c r="B6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>71</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>32</v>
@@ -916,33 +929,35 @@
         <v>37</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>43</v>
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <f t="shared" ref="A9:A25" si="1">ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="F9" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>43</v>
@@ -951,78 +966,76 @@
     </row>
     <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A10:A26" si="1">ROW()-1</f>
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>43</v>
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>8</v>
+        <v>57</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>32</v>
+        <v>56</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
@@ -1030,171 +1043,173 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>8</v>
+        <v>55</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>30</v>
+        <v>52</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>8</v>
+        <v>39</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>64</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="F17" s="2" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="H17" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>8</v>
+        <v>29</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="2"/>
+      <c r="D19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="1"/>
       <c r="F19" s="2" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -1203,21 +1218,21 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -1226,21 +1241,21 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -1249,53 +1264,53 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>8</v>
@@ -1305,20 +1320,20 @@
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>8</v>
@@ -1328,22 +1343,35 @@
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
@@ -1405,9 +1433,19 @@
       <c r="G32" s="2"/>
       <c r="H32" s="1"/>
     </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="1"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H32">
-    <sortCondition descending="1" ref="B17:B32"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H33">
+    <sortCondition descending="1" ref="B18:B33"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
BUG0003:Runtime error during docker-compose up --build was crashing frontend container. Error was reportde at: /app/node_modules/path-to-regexp/dist/index.js:73 throw new TypeError(Missing parameter name at : );BUG0004:The ready-to-use commands were not automatically getting updated with the first company name after the dropdown was updated with active companies.
</commit_message>
<xml_diff>
--- a/LLM/EquityResearchReports/ER_Change_History.xlsx
+++ b/LLM/EquityResearchReports/ER_Change_History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shriniwasiyengar/git/python_ML/LLM/EquityResearchReports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C278662-771B-2E4A-BEC0-C66B62E6266D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AC9659-7130-8F42-A95E-617E7573084A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{F111C49C-E983-B94D-AD50-206753B053C1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="97">
   <si>
     <t>CR or Bug #</t>
   </si>
@@ -323,6 +323,36 @@
   </si>
   <si>
     <t>Created additional endpoints in Sources Management Service. Added new event for getting companies list. Added separate Sources_URL environment variable.</t>
+  </si>
+  <si>
+    <t>BUG0003</t>
+  </si>
+  <si>
+    <t>Runtime error during docker-compose up --build was crashing frontend container. Error was reportde at: /app/node_modules/path-to-regexp/dist/index.js:73 throw new TypeError(Missing parameter name at ${i}: ${DEBUG_URL})</t>
+  </si>
+  <si>
+    <t>Error was apparently due to (automatic) upgradation of express.js to 5.xx which uses different syntax for parsing the app.use(express.static(path.join(__dirname, 'dist/frontend'))); cmmand used in server.js. The solution was to downgrade express.js to 4.21.x by changing the express install command in Dockerfile-frontend to: RUN npm install express@4.21.2.</t>
+  </si>
+  <si>
+    <t>The ready-to-use commands were not automatically getting updated with the first company name after the dropdown was updated with active companies.</t>
+  </si>
+  <si>
+    <t>Added this.updateCommands() to the loadCompanies method in chat.component.ts to force an update to the commands whenever the companies dropdown is updated.</t>
+  </si>
+  <si>
+    <t>BUG0004</t>
+  </si>
+  <si>
+    <t>BUG0005</t>
+  </si>
+  <si>
+    <t>The tab should switch to Chat if user clicks on a ready-to-use command when another tab (for example, sources tab) is in focus.</t>
+  </si>
+  <si>
+    <t>CR0024</t>
+  </si>
+  <si>
+    <t>Add "Activate" button to sources CRUD listing so that users can activate an inactive source. This will require a check on whether a PDF file is already associated with the company or not. Also, user can choose to change the PDF if necessary during activation.</t>
   </si>
 </sst>
 </file>
@@ -728,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3DE150-7B8A-A542-8341-29F2F94982DD}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -770,124 +800,126 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
-        <f t="shared" ref="A2:A9" si="0">ROW()-1</f>
+        <f t="shared" ref="A2:A13" si="0">ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>8</v>
+      <c r="B2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+        <v>43</v>
+      </c>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>81</v>
+      <c r="B3" s="8" t="s">
+        <v>93</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="D3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="B4" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="E4" s="8"/>
+      <c r="F4" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="D5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="3"/>
+      <c r="B6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
@@ -895,24 +927,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
+        <v>81</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="E7" s="3"/>
       <c r="F7" s="2" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
@@ -920,24 +950,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E8" s="3"/>
       <c r="F8" s="2" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
@@ -945,32 +973,32 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>32</v>
+        <v>76</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>77</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E9" s="3"/>
       <c r="F9" s="2" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <f t="shared" ref="A10:A26" si="1">ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>32</v>
@@ -978,84 +1006,84 @@
       <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="2" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>32</v>
+        <v>71</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>8</v>
+        <v>60</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>43</v>
@@ -1064,176 +1092,178 @@
     </row>
     <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A14:A30" si="1">ROW()-1</f>
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>8</v>
+        <v>67</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>51</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>30</v>
+        <v>57</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>32</v>
+        <v>56</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <f>ROW()-1</f>
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="F18" s="2" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="F19" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>8</v>
+        <v>39</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="F20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
@@ -1241,76 +1271,80 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="F21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="H21" s="2" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="1"/>
       <c r="F22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="1"/>
       <c r="F23" s="2" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>8</v>
@@ -1320,43 +1354,43 @@
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>8</v>
@@ -1366,52 +1400,104 @@
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
@@ -1443,9 +1529,49 @@
       <c r="G33" s="2"/>
       <c r="H33" s="1"/>
     </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="2"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="2"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="1"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H33">
-    <sortCondition descending="1" ref="B18:B33"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:H37">
+    <sortCondition descending="1" ref="B22:B37"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Initial commits for CR0033 and CR0030
</commit_message>
<xml_diff>
--- a/LLM/EquityResearchReports/ER_Change_History.xlsx
+++ b/LLM/EquityResearchReports/ER_Change_History.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shriniwasiyengar/git/python_ML/LLM/EquityResearchReports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AC9659-7130-8F42-A95E-617E7573084A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B412289C-4DE1-AC44-A091-55700122179A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{F111C49C-E983-B94D-AD50-206753B053C1}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19940" xr2:uid="{F111C49C-E983-B94D-AD50-206753B053C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="119">
   <si>
     <t>CR or Bug #</t>
   </si>
@@ -283,12 +283,6 @@
     <t>Add ability to generate templatized Investment Analysis Report. Display this report in a tab.</t>
   </si>
   <si>
-    <t>Add ability to create template for IA Report containing sections and questions or directives for retrieving data for the sections from source documents.</t>
-  </si>
-  <si>
-    <t>CR0020</t>
-  </si>
-  <si>
     <t>Add ability to upload, associate and process multiple source files for each company.</t>
   </si>
   <si>
@@ -352,14 +346,87 @@
     <t>CR0024</t>
   </si>
   <si>
-    <t>Add "Activate" button to sources CRUD listing so that users can activate an inactive source. This will require a check on whether a PDF file is already associated with the company or not. Also, user can choose to change the PDF if necessary during activation.</t>
+    <t>CR0025</t>
+  </si>
+  <si>
+    <t>CR0026</t>
+  </si>
+  <si>
+    <t>IA Report</t>
+  </si>
+  <si>
+    <t>Sources Management</t>
+  </si>
+  <si>
+    <t>Add ability to download template for IA report as PDF</t>
+  </si>
+  <si>
+    <t>CR0027</t>
+  </si>
+  <si>
+    <t>Add ability to specify multiple PDFs as sources for a company.</t>
+  </si>
+  <si>
+    <t>Add ability to specify template for IA report containing sections and questions or directives for retrieving data for the sections from source documents.</t>
+  </si>
+  <si>
+    <t>Show sources and update RAGA metrics for data retrieved in IA report</t>
+  </si>
+  <si>
+    <t>Add "Activate" button to sources CRUD listing so that users can activate an inactive source. This will require a check on whether a PDF file is already associated with the company or not. Also, user can choose to change the PDF if necessary during activation.This action should also add the company to the company-selector dropdown.
+Also add a "Deactivate" button to deactivate an existing source. This action should also remove the company from the company-selector dropdown.</t>
+  </si>
+  <si>
+    <t>Create LSTM modules (training and forecasting) for predicting future values of stock prices</t>
+  </si>
+  <si>
+    <t>Create Seq2Seq modules (training and forecasting) for predicting future values of stock prices</t>
+  </si>
+  <si>
+    <t>Extend LSTM modules to handle multiple stocks</t>
+  </si>
+  <si>
+    <t>Extend Seq2Seq modules to handle multiple stocks</t>
+  </si>
+  <si>
+    <t>Create local datastore to replace raw CSV files being used currently for ML models and analytics</t>
+  </si>
+  <si>
+    <t>CR0028</t>
+  </si>
+  <si>
+    <t>CR0029</t>
+  </si>
+  <si>
+    <t>CR0030</t>
+  </si>
+  <si>
+    <t>CR0031</t>
+  </si>
+  <si>
+    <t>CR0032</t>
+  </si>
+  <si>
+    <t>CR0033</t>
+  </si>
+  <si>
+    <t>CR0034</t>
+  </si>
+  <si>
+    <t>AI Service</t>
+  </si>
+  <si>
+    <t>Integrate LSTM predictor into Angular UI using plotly and flask</t>
+  </si>
+  <si>
+    <t>Integrate Seq2Seq predictor into Angular UI using plotly and flask</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -371,6 +438,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -440,10 +514,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3DE150-7B8A-A542-8341-29F2F94982DD}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -800,157 +874,151 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="8">
-        <f t="shared" ref="A2:A13" si="0">ROW()-1</f>
+    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <f t="shared" ref="A2:A8" si="0">ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>95</v>
+      <c r="B2" s="10" t="s">
+        <v>115</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="8"/>
+      <c r="D2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>116</v>
+      </c>
       <c r="F2" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="1:8" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="8">
+        <v>108</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="8"/>
+      <c r="B3" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>116</v>
+      </c>
       <c r="F3" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>43</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="G3" s="8"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="8">
+    <row r="4" spans="1:8" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="8"/>
+      <c r="B4" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>116</v>
+      </c>
       <c r="F4" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="8">
+        <v>117</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="1:8" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="8"/>
+      <c r="B5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>116</v>
+      </c>
       <c r="F5" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="8">
+        <v>106</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="8"/>
+      <c r="B6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>116</v>
+      </c>
       <c r="F6" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>110</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>32</v>
@@ -958,47 +1026,47 @@
       <c r="D8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="E8" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A9:A23" si="1">ROW()-1</f>
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>8</v>
+        <v>99</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="F9" s="2" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>32</v>
@@ -1006,143 +1074,147 @@
       <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="F10" s="2" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>46</v>
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>8</v>
+        <v>94</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="F11" s="2" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>43</v>
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <f t="shared" ref="A14:A30" si="1">ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>43</v>
       </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>32</v>
+        <v>90</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>8</v>
@@ -1150,17 +1222,15 @@
       <c r="D16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -1169,101 +1239,95 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>32</v>
+        <v>82</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>54</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>8</v>
+        <v>79</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="E18" s="3"/>
       <c r="F18" s="2" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>30</v>
+        <v>76</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="E19" s="3"/>
       <c r="F19" s="2" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>32</v>
+        <v>74</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>40</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E20" s="3"/>
       <c r="F20" s="2" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
@@ -1271,126 +1335,128 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <f>ROW()-1</f>
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="1"/>
       <c r="F22" s="2" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="F23" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A24:A40" si="2">ROW()-1</f>
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>8</v>
+        <v>67</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>8</v>
+        <v>57</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>8</v>
@@ -1398,45 +1464,51 @@
       <c r="D26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="F26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="H26" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>18</v>
+        <v>55</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="F27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>8</v>
@@ -1444,134 +1516,376 @@
       <c r="D28" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="F28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G28" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="H28" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>8</v>
+        <v>53</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E29" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="F29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>8</v>
+        <v>39</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="F30" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <f>ROW()-1</f>
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2" t="s">
+      <c r="G40" s="2"/>
+      <c r="H40" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="1"/>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="2"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="2"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="2"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="2"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="2"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="2"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:H37">
-    <sortCondition descending="1" ref="B22:B37"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:H47">
+    <sortCondition descending="1" ref="B32:B47"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CR0034, CR0035, CR0036: Added stock-data-viewer, stock-data and Api-gatway services
</commit_message>
<xml_diff>
--- a/LLM/EquityResearchReports/ER_Change_History.xlsx
+++ b/LLM/EquityResearchReports/ER_Change_History.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shriniwasiyengar/git/python_ML/LLM/EquityResearchReports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B412289C-4DE1-AC44-A091-55700122179A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A52108-A71C-0048-9B06-EF2F76F176E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19940" xr2:uid="{F111C49C-E983-B94D-AD50-206753B053C1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="123">
   <si>
     <t>CR or Bug #</t>
   </si>
@@ -420,6 +420,18 @@
   </si>
   <si>
     <t>Integrate Seq2Seq predictor into Angular UI using plotly and flask</t>
+  </si>
+  <si>
+    <t>CR0035</t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
+    <t>Add API-gateway for dynamic discovery of microservices</t>
+  </si>
+  <si>
+    <t>Use Consul and Spring Clould API gatewy to avoid hardwiding IP addresses and port numbers in individual service configs, Dockerfiles etc.</t>
   </si>
 </sst>
 </file>
@@ -488,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -511,11 +523,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -832,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3DE150-7B8A-A542-8341-29F2F94982DD}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -875,58 +886,59 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <f t="shared" ref="A2:A8" si="0">ROW()-1</f>
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <f t="shared" ref="A3:A9" si="0">ROW()-1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E3" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F3" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-    </row>
-    <row r="4" spans="1:8" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>113</v>
+      <c r="B4" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>30</v>
@@ -934,68 +946,68 @@
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-    </row>
-    <row r="5" spans="1:8" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="F4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>32</v>
+      <c r="B5" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="F5" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>30</v>
+        <v>112</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="1:8" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="F6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>30</v>
@@ -1003,45 +1015,45 @@
       <c r="D7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" spans="1:8" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="F7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>32</v>
+        <v>110</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="F8" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <f t="shared" ref="A9:A23" si="1">ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>32</v>
@@ -1050,23 +1062,21 @@
         <v>38</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="3"/>
+        <v>107</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A10:A24" si="1">ROW()-1</f>
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>32</v>
@@ -1078,10 +1088,10 @@
         <v>96</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H10" s="3"/>
     </row>
@@ -1091,7 +1101,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>32</v>
@@ -1103,20 +1113,20 @@
         <v>96</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>46</v>
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>32</v>
@@ -1128,20 +1138,20 @@
         <v>96</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>46</v>
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>32</v>
@@ -1150,33 +1160,35 @@
         <v>38</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="F14" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>43</v>
@@ -1189,57 +1201,55 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>8</v>
+        <v>91</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>8</v>
@@ -1249,85 +1259,85 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>32</v>
+        <v>82</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>46</v>
       </c>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>8</v>
+        <v>76</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>80</v>
-      </c>
+      <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
@@ -1335,7 +1345,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>8</v>
@@ -1343,49 +1353,49 @@
       <c r="D21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="3"/>
       <c r="F21" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>46</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>32</v>
+        <v>71</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>32</v>
@@ -1394,33 +1404,35 @@
         <v>37</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>43</v>
       </c>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <f t="shared" ref="A24:A40" si="2">ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="F24" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>43</v>
@@ -1429,78 +1441,76 @@
     </row>
     <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A25:A41" si="2">ROW()-1</f>
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>43</v>
       </c>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>8</v>
+        <v>57</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>32</v>
+        <v>56</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H27" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
@@ -1508,171 +1518,173 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>8</v>
+        <v>55</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>30</v>
+        <v>52</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>8</v>
+        <v>39</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>64</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E32" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="F32" s="2" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="H32" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>8</v>
+        <v>29</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E34" s="2"/>
+      <c r="D34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="1"/>
       <c r="F34" s="2" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -1681,21 +1693,21 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -1704,21 +1716,21 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -1727,53 +1739,53 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>8</v>
@@ -1783,20 +1795,20 @@
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>8</v>
@@ -1806,22 +1818,35 @@
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
@@ -1883,9 +1908,19 @@
       <c r="G47" s="2"/>
       <c r="H47" s="1"/>
     </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="2"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="1"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:H47">
-    <sortCondition descending="1" ref="B32:B47"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A19:H48">
+    <sortCondition descending="1" ref="B33:B48"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>